<commit_message>
unique values for GEOME fields
</commit_message>
<xml_diff>
--- a/examples/GEOME/requiredFieldsWork.xlsx
+++ b/examples/GEOME/requiredFieldsWork.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\examples\GEOME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5994D262-7130-4700-8FE7-27614616CB11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421B4847-7C81-414E-87C8-AED1DF97A4C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1275" windowWidth="22020" windowHeight="14325" activeTab="1"/>
+    <workbookView xWindow="4350" yWindow="1920" windowWidth="21315" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summaryStart" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1364,7 +1364,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1869"/>
   <sheetViews>
     <sheetView topLeftCell="A253" workbookViewId="0">
@@ -27546,7 +27546,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1870"/>
+  <autoFilter ref="A1:D1870" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1869">
     <sortCondition ref="B2:B1869"/>
     <sortCondition ref="D2:D1869"/>
@@ -27556,11 +27556,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27589,63 +27589,63 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>145</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -27653,7 +27653,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -27661,7 +27661,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -27669,7 +27669,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -27677,7 +27677,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -27685,47 +27685,53 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -27746,177 +27752,180 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>142</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>152</v>
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -27924,26 +27933,23 @@
         <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -27951,26 +27957,23 @@
         <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -27978,18 +27981,18 @@
         <v>9</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -28019,24 +28022,24 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -28044,49 +28047,46 @@
         <v>36</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C56">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E56">
+    <sortCondition ref="B2:B56"/>
     <sortCondition ref="A2:A56"/>
-    <sortCondition ref="B2:B56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Geome fields and mapping
</commit_message>
<xml_diff>
--- a/examples/GEOME/requiredFieldsWork.xlsx
+++ b/examples/GEOME/requiredFieldsWork.xlsx
@@ -1,30 +1,456 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\examples\GEOME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421B4847-7C81-414E-87C8-AED1DF97A4C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF473A0-9BD8-45D5-9B97-440F3029A28D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="1920" windowWidth="21315" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="1725" windowWidth="15195" windowHeight="14250" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summaryStart" sheetId="1" r:id="rId1"/>
-    <sheet name="UniqueValues" sheetId="2" r:id="rId2"/>
+    <sheet name="All required columns" sheetId="3" r:id="rId2"/>
+    <sheet name="EventColumns" sheetId="4" r:id="rId3"/>
+    <sheet name="SampleColumns" sheetId="5" r:id="rId4"/>
+    <sheet name="DiagnosticsColumns" sheetId="6" r:id="rId5"/>
+    <sheet name="TissueColumns" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EventColumns!$B$1:$B$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">summaryStart!$A$1:$D$1870</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Stephen Richard</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{ED1E6B16-6ACB-4692-B8D3-6604EA396846}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The full name of the lithostratigraphic bed from which the cataloged item was collected.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{43A738C5-2997-498B-8A50-B9C59B9638C4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The names of the cultural groups with which the occupants of the site would have been affiliated during the occupational period to which these specimens pertain - these are modern names where original culture names are unknown.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{2FFDF1BE-1A72-4B03-B76C-175F8FD4D905}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The culturally defined region or regions of which this site was a part during the occupational period to which these specimens pertain - spatially or spatio-temporally defined.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{17497B20-C224-45EB-BF10-847B83285A1F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>terms that identify the material displaced by the entity at time of sampling. Recommend subclasses of environmental material http://purl.obolibrary.org/obo/ENVO_00010483</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{DD1DFC0E-B7AE-48DF-9130-EEF04611D7FF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The full name of the lithostratigraphic formation from which the cataloged item was collected.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{E2C0BAD5-140C-4ABC-8682-609C4D3244C6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An identifier for the set of information associated with a GeologicalContext (the location within a geological context, such as stratigraphy). May be a global unique identifier or an identifier specific to the data set.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{FF882C6F-99CA-4786-89BE-3CB7E9BA9A3A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The full name of the lithostratigraphic group from which the cataloged item was collected.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A49" authorId="0" shapeId="0" xr:uid="{C841E628-2BBE-46FE-AC35-4E82A892C133}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The combination of all litho-stratigraphic names for the rock from which the cataloged item was collected.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{69D861B2-8665-494E-AE7E-360F1A8A5048}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Substrate from which the individual was sampled. This could be abiotic or biotic (host organism).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A71" authorId="0" shapeId="0" xr:uid="{17B7DB97-1F4E-4CCC-9E00-1D584BA79657}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The taxonomic team.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Stephen Richard</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5BD01C06-4ACF-42DD-A3B7-8544BD8664AB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Photos, videos etc of the individual. From Darwincore: A list (concatenated and separated) of identifiers (publication, global unique identifier, URI,DOI) of media associated with the Occurrence.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{4EC38C09-97AC-4CD3-A8D3-BE5213930422}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The specific nature of the data record.  Examples include PreservedSpecimen, FossilSpecimen, LivingSpecimen, MaterialSample, Event, HumanObservation, MachineObservation, Taxon, Occurrence</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{A292817E-A316-4EC6-B325-D832CEEE9F8F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>unique codes automatically generated for each new record added to a project within the Barcode of Life Database. They serve to connect specimen information, such as taxonomy, collection data and images, to the DNA barcode sequence for that specimen.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{1E4F74CB-EE8F-4BA2-B2D7-F464ED1A2A06}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The full scientific name of the class in which the taxon is classified</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{0208210E-5787-4662-8D5D-AB1D8852A7B9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A common or venacular name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{C458E9D0-67F5-4411-A2E9-019F0F18C2FB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The name identifying the data set from which the record was derived.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{A22EB3D2-1C22-4F1B-A26D-AEECD0DF2969}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A list of additional measurements, facts, characteristics, or assertions about the record. Meant to provide a mechanism for structured content.  Recommended best practice is to use a key:value encoding schema for a data interchange format such as JSON.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{02CACFDA-04D9-4356-8705-31F01130480C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The process by which the biological individual(s) represented in the Occurrence became established at the location. Recommended best practice is to use a controlled vocabulary. See associated list in lists tab.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{E6D03C7F-F924-4CE2-B8A0-27D99087260C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A field to populate the /specimen_voucher qualifier field for submissions to Genbank.  Please refer to the instructions for populating /specimen_voucher at the &lt;a href='https://www.ncbi.nlm.nih.gov/books/NBK53701/'&gt;Genbank Submission Handbook</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{F22EAB9C-E145-4DDA-983D-3C71A7792B9C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>An identifier of a distinct individual (e.g. all bones within the same associated skeleton would have the same individualID).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{1A9ED1DC-B056-4B4B-B65E-117093C0D1A4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The third word in the scientific name of an infraspecific taxon, following the name of the species. This applies only to formal names of plants and fungi, and not to the formal names of bacteria or animals.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{02B0006C-EF28-409F-ACF0-9738C8706E3A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The name (or acronym) in use by the institution having custody of the object(s) or information referred to in the record.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{02694076-D448-4E4A-A2AF-E1A3B62A0E44}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identifiers of other organisms which match the mortphospeciesDescription</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="0" shapeId="0" xr:uid="{88E249DA-588C-416B-A4E6-96B9455A39CB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The name of a particular individual.  For example, if there is a Kiwi called 'Freddy', we would put 'Freddy' in the nameOfIndividual Field. This is common practice in Mauri culture to name specific individuals. Note that this is NOT the same as vernacularName</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{62760569-B8D9-4E62-B61C-79C12AAC91B7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The nomenclatural code (or codes in the case of an ambiregnal name) under which the scientificName is constructed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A47" authorId="0" shapeId="0" xr:uid="{D41A34C7-01B7-42D7-9760-AA4714054934}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">An identifier for the Organism instance.  Can refer to a lot or a single specimen or a single individual of the same taxon.  This identifier does not guarrantee that we are referring to a distinct individual. May be a globally unique identifier or an identifier specific to the data set. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{C868859C-E2AE-47B9-93A3-1EE01516C63F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A related resource that is referenced, cited, or otherwise pointed to by the described resource.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A75" authorId="0" shapeId="0" xr:uid="{FEB7C983-3DE5-4B7C-8414-CDC6B23997CE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> a visible notification that there is accompanying cultural rights and responsibilities that need further attention for any future sharing and use of this material. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Stephen Richard</author>
+  </authors>
+  <commentList>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{AC4C5A15-9190-46C3-B980-EC392FDA3E14}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sample or specimen data can not be ordered/loaned in general, but are visible via portals. Accepts TRUE or FALSE.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5741" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6109" uniqueCount="367">
   <si>
     <t>record_alias</t>
   </si>
@@ -452,58 +878,679 @@
     <t>USGS National Survey for the Amphibian Chytrid Fungus Batrachochytrium salamandrivorans</t>
   </si>
   <si>
-    <t>FK to Event</t>
-  </si>
-  <si>
-    <t>FK to Sample</t>
-  </si>
-  <si>
-    <t>PK</t>
-  </si>
-  <si>
-    <t>FK to sample</t>
-  </si>
-  <si>
-    <t>FK to photo</t>
-  </si>
-  <si>
-    <t>FK to Photo</t>
-  </si>
-  <si>
-    <t>FK to Tissue</t>
-  </si>
-  <si>
-    <t>The well location in the plate</t>
-  </si>
-  <si>
-    <t>The name of the plate. Typically this is a 96 well plat for Biocode projects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The plate  can be considered a sample collection; analogs-- microprobe point in a thin section, mineral grain in a grain mount; </t>
-  </si>
-  <si>
-    <t>The specific nature of the data record. Examples include PreservedSpecimen, FossilSpecimen, LivingSpecimen, MaterialSample, Event, HumanObservation, MachineObservation, Taxon, Occurrence.  "group": "Taxonomy and Life History"</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>The full scientific name of the specificEpithet (the second element in the Latin binomial name of a species) in which the taxon is classified</t>
-  </si>
-  <si>
-    <t>Epithet-the second element in the Latin binomial name of a species, which follows the generic name and distinguishes the species from others in the same genus.</t>
-  </si>
-  <si>
-    <t>scientificName as the lowest taxon identified</t>
-  </si>
-  <si>
-    <t>A designation of a child projecct within the larger project.</t>
+    <t>bed</t>
+  </si>
+  <si>
+    <t>chronometricAgeID</t>
+  </si>
+  <si>
+    <t>chronometricAgeProtocol</t>
+  </si>
+  <si>
+    <t>chronometricAgeUncertaintyInYears</t>
+  </si>
+  <si>
+    <t>chronometricAgeUncertaintyMethod</t>
+  </si>
+  <si>
+    <t>continentOcean</t>
+  </si>
+  <si>
+    <t>coordinatePrecision</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>culturalAffiliations</t>
+  </si>
+  <si>
+    <t>culturalContext</t>
+  </si>
+  <si>
+    <t>culturalOccupationPeriod</t>
+  </si>
+  <si>
+    <t>culturalRegions</t>
+  </si>
+  <si>
+    <t>dayCollected</t>
+  </si>
+  <si>
+    <t>decimalLatitudeEnd</t>
+  </si>
+  <si>
+    <t>decimalLongitudeEnd</t>
+  </si>
+  <si>
+    <t>depthOfBottomInMeters</t>
+  </si>
+  <si>
+    <t>earliestAgeOrLowestStage</t>
+  </si>
+  <si>
+    <t>earliestEonOrLowestEonothem</t>
+  </si>
+  <si>
+    <t>earliestEpochOrLowestSeries</t>
+  </si>
+  <si>
+    <t>earliestEraOrLowestErathem</t>
+  </si>
+  <si>
+    <t>earliestPeriodOrLowestSystem</t>
+  </si>
+  <si>
+    <t>environmentalMedium</t>
+  </si>
+  <si>
+    <t>eventRemarks</t>
+  </si>
+  <si>
+    <t>fieldNotes</t>
+  </si>
+  <si>
+    <t>formation</t>
+  </si>
+  <si>
+    <t>fundingSource</t>
+  </si>
+  <si>
+    <t>geologicalContextID</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>highestBiostratigraphicZone</t>
+  </si>
+  <si>
+    <t>horizontalDatum</t>
+  </si>
+  <si>
+    <t>island</t>
+  </si>
+  <si>
+    <t>islandGroup</t>
+  </si>
+  <si>
+    <t>landowner</t>
+  </si>
+  <si>
+    <t>latestAgeOrHighestStage</t>
+  </si>
+  <si>
+    <t>latestEonOrHighestEonotheme</t>
+  </si>
+  <si>
+    <t>latestEpochOrHighestSeries</t>
+  </si>
+  <si>
+    <t>latestEraOrHighestErathem</t>
+  </si>
+  <si>
+    <t>latestPeriodOrHighestSystem</t>
+  </si>
+  <si>
+    <t>lithostratigraphicTerms</t>
+  </si>
+  <si>
+    <t>locationID</t>
+  </si>
+  <si>
+    <t>locationRemarks</t>
+  </si>
+  <si>
+    <t>lowestBiostratigraphicZone</t>
+  </si>
+  <si>
+    <t>maximumChronometricAge</t>
+  </si>
+  <si>
+    <t>maximumChronometricAgeReferenceSystem</t>
+  </si>
+  <si>
+    <t>maximumDepthInMeters</t>
+  </si>
+  <si>
+    <t>maximumElevationInMeters</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>microHabitat</t>
+  </si>
+  <si>
+    <t>minimumChronometricAge</t>
+  </si>
+  <si>
+    <t>minimumChronometricAgeReferenceSystem</t>
+  </si>
+  <si>
+    <t>minimumDepthInMeters</t>
+  </si>
+  <si>
+    <t>minimumElevationInMeters</t>
+  </si>
+  <si>
+    <t>monthCollected</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>permitInformation</t>
+  </si>
+  <si>
+    <t>stateProvince</t>
+  </si>
+  <si>
+    <t>substratum</t>
+  </si>
+  <si>
+    <t>taxTeam</t>
+  </si>
+  <si>
+    <t>timeOfDay</t>
+  </si>
+  <si>
+    <t>verbatimDepth</t>
+  </si>
+  <si>
+    <t>verbatimElevation</t>
+  </si>
+  <si>
+    <t>verbatimEventDate</t>
+  </si>
+  <si>
+    <t>verbatimLatitude</t>
+  </si>
+  <si>
+    <t>verbatimLocality</t>
+  </si>
+  <si>
+    <t>verbatimLongitude</t>
+  </si>
+  <si>
+    <t>waterBody</t>
+  </si>
+  <si>
+    <t>associatedMedia</t>
+  </si>
+  <si>
+    <t>associatedReferences</t>
+  </si>
+  <si>
+    <t>associatedTaxa</t>
+  </si>
+  <si>
+    <t>boldProcessID</t>
+  </si>
+  <si>
+    <t>catalogNumber</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>collectionCode</t>
+  </si>
+  <si>
+    <t>colloquialName</t>
+  </si>
+  <si>
+    <t>datasetName</t>
+  </si>
+  <si>
+    <t>dayIdentified</t>
+  </si>
+  <si>
+    <t>dynamicProperties</t>
+  </si>
+  <si>
+    <t>establishmentMeans</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>fieldNumber</t>
+  </si>
+  <si>
+    <t>fixative</t>
+  </si>
+  <si>
+    <t>genbankSpecimenVoucher</t>
+  </si>
+  <si>
+    <t>identificationRemarks</t>
+  </si>
+  <si>
+    <t>identificationVerificationStatus</t>
+  </si>
+  <si>
+    <t>identifiedBy</t>
+  </si>
+  <si>
+    <t>individualCount</t>
+  </si>
+  <si>
+    <t>individualID</t>
+  </si>
+  <si>
+    <t>informationWithheld</t>
+  </si>
+  <si>
+    <t>infraClass</t>
+  </si>
+  <si>
+    <t>infraOrder</t>
+  </si>
+  <si>
+    <t>infraspecificEpithet</t>
+  </si>
+  <si>
+    <t>institutionID</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>lengthUnits</t>
+  </si>
+  <si>
+    <t>lifeStage</t>
+  </si>
+  <si>
+    <t>modifiedBy</t>
+  </si>
+  <si>
+    <t>modifiedReason</t>
+  </si>
+  <si>
+    <t>monthIdentified</t>
+  </si>
+  <si>
+    <t>morphospeciesDescription</t>
+  </si>
+  <si>
+    <t>morphospeciesMatch</t>
+  </si>
+  <si>
+    <t>nameOfIndividual</t>
+  </si>
+  <si>
+    <t>nomenclaturalCode</t>
+  </si>
+  <si>
+    <t>occurrenceID</t>
+  </si>
+  <si>
+    <t>occurrenceRemarks</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>organismID</t>
+  </si>
+  <si>
+    <t>organismQuantity</t>
+  </si>
+  <si>
+    <t>organismQuantityType</t>
+  </si>
+  <si>
+    <t>organismRemarks</t>
+  </si>
+  <si>
+    <t>otherCatalogNumbers</t>
+  </si>
+  <si>
+    <t>preparationType</t>
+  </si>
+  <si>
+    <t>preservative</t>
+  </si>
+  <si>
+    <t>previousIdentifications</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>relaxant</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>subClass</t>
+  </si>
+  <si>
+    <t>subFamily</t>
+  </si>
+  <si>
+    <t>subGenus</t>
+  </si>
+  <si>
+    <t>subOrder</t>
+  </si>
+  <si>
+    <t>subPhylum</t>
+  </si>
+  <si>
+    <t>subSubProject</t>
+  </si>
+  <si>
+    <t>subTribe</t>
+  </si>
+  <si>
+    <t>superClass</t>
+  </si>
+  <si>
+    <t>superFamily</t>
+  </si>
+  <si>
+    <t>superOrder</t>
+  </si>
+  <si>
+    <t>taxonRank</t>
+  </si>
+  <si>
+    <t>taxonRemarks</t>
+  </si>
+  <si>
+    <t>traditionalKnowledgeNotice</t>
+  </si>
+  <si>
+    <t>tribe</t>
+  </si>
+  <si>
+    <t>typeStatus</t>
+  </si>
+  <si>
+    <t>verbatimLifeStage</t>
+  </si>
+  <si>
+    <t>voucherCatalogNumber</t>
+  </si>
+  <si>
+    <t>voucherURI</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>weightUnits</t>
+  </si>
+  <si>
+    <t>wormsID</t>
+  </si>
+  <si>
+    <t>yearIdentified</t>
+  </si>
+  <si>
+    <t>ageEstimationMethod</t>
+  </si>
+  <si>
+    <t>ageUnit</t>
+  </si>
+  <si>
+    <t>ageValue</t>
+  </si>
+  <si>
+    <t>cycleTimeFirstDetection</t>
+  </si>
+  <si>
+    <t>diagnosticLab</t>
+  </si>
+  <si>
+    <t>dilutionFactor</t>
+  </si>
+  <si>
+    <t>diseaseLineage</t>
+  </si>
+  <si>
+    <t>diseaseTestedPositiveCount</t>
+  </si>
+  <si>
+    <t>genotypeMethod</t>
+  </si>
+  <si>
+    <t>materialSampleCondition</t>
+  </si>
+  <si>
+    <t>materialSampleType</t>
+  </si>
+  <si>
+    <t>measurementAccuracy</t>
+  </si>
+  <si>
+    <t>measurementDeterminedBy</t>
+  </si>
+  <si>
+    <t>measurementDeterminedDate</t>
+  </si>
+  <si>
+    <t>measurementMethodURI</t>
+  </si>
+  <si>
+    <t>measurementRemarks</t>
+  </si>
+  <si>
+    <t>measurementSide</t>
+  </si>
+  <si>
+    <t>quantityDetected</t>
+  </si>
+  <si>
+    <t>reproductiveCondition</t>
+  </si>
+  <si>
+    <t>specimenDisposition</t>
+  </si>
+  <si>
+    <t>testMethod</t>
+  </si>
+  <si>
+    <t>verbatimAgeValue</t>
+  </si>
+  <si>
+    <t>zeScore</t>
+  </si>
+  <si>
+    <t>associatedSequences</t>
+  </si>
+  <si>
+    <t>biosampleAccession</t>
+  </si>
+  <si>
+    <t>fromTissue</t>
+  </si>
+  <si>
+    <t>tissueBarcode</t>
+  </si>
+  <si>
+    <t>tissueBlocked</t>
+  </si>
+  <si>
+    <t>tissueCatalogNumber</t>
+  </si>
+  <si>
+    <t>tissueContainer</t>
+  </si>
+  <si>
+    <t>tissueInstitution</t>
+  </si>
+  <si>
+    <t>tissueOtherCatalogNumbers</t>
+  </si>
+  <si>
+    <t>tissuePreservative</t>
+  </si>
+  <si>
+    <t>tissueRecordedBy</t>
+  </si>
+  <si>
+    <t>tissueRemarks</t>
+  </si>
+  <si>
+    <t>tissueSamplingDay</t>
+  </si>
+  <si>
+    <t>tissueSamplingMonth</t>
+  </si>
+  <si>
+    <t>tissueSamplingYear</t>
+  </si>
+  <si>
+    <t>tissueType</t>
+  </si>
+  <si>
+    <t>related resource</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent </t>
+  </si>
+  <si>
+    <t>altID</t>
+  </si>
+  <si>
+    <t>curation</t>
+  </si>
+  <si>
+    <t>curationLocation</t>
+  </si>
+  <si>
+    <t>registrant</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>samplingEvent.date</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>accessConstraints</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>samplingEvent.responsibleParty</t>
+  </si>
+  <si>
+    <t>samplingSite.placeName</t>
+  </si>
+  <si>
+    <t>GeospatialLocation.positionUncertainty</t>
+  </si>
+  <si>
+    <t>GeospatialDDCoordLocation</t>
+  </si>
+  <si>
+    <t>GeospatialLocation.</t>
+  </si>
+  <si>
+    <t>GeospatialLocation</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>initiative.responsibility</t>
+  </si>
+  <si>
+    <t>map to sampled feature?</t>
+  </si>
+  <si>
+    <t>samplingSite.identifier</t>
+  </si>
+  <si>
+    <t>samplingSite.description</t>
+  </si>
+  <si>
+    <t>samplingMethod</t>
+  </si>
+  <si>
+    <t>samplingEvent.responsibility</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>iSampleMapping</t>
+  </si>
+  <si>
+    <t>context--chrono</t>
+  </si>
+  <si>
+    <t>context--stratigraphic</t>
+  </si>
+  <si>
+    <t>context--cultural</t>
+  </si>
+  <si>
+    <t>context--environmental</t>
+  </si>
+  <si>
+    <t>relatedResource</t>
+  </si>
+  <si>
+    <t>specimenType</t>
+  </si>
+  <si>
+    <t>isPartOf.SampleCollection</t>
+  </si>
+  <si>
+    <t>category:taxonomy</t>
+  </si>
+  <si>
+    <t>informal classification</t>
+  </si>
+  <si>
+    <t>history.Event</t>
+  </si>
+  <si>
+    <t>additionalProperty</t>
+  </si>
+  <si>
+    <t>samplingEvent.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initiative </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>context:chrono</t>
+  </si>
+  <si>
+    <t>sample identifier</t>
+  </si>
+  <si>
+    <t>specimen type</t>
+  </si>
+  <si>
+    <t>PropertyValue</t>
+  </si>
+  <si>
+    <t>material type, specimen type</t>
+  </si>
+  <si>
+    <t>related to measurement, not sample</t>
   </si>
 </sst>
 </file>
@@ -646,10 +1693,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0B7500"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -993,7 +2040,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1001,14 +2048,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="4" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1367,8 +2408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1869"/>
   <sheetViews>
-    <sheetView topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="A253" sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D270" sqref="D270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27556,539 +28597,2135 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8057751-A5D6-43C2-B0FC-9024D1FECCB9}">
+  <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.5703125" customWidth="1"/>
-    <col min="5" max="5" width="42" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A472B710-19EE-4903-8EC9-3BCEC24609CC}">
+  <dimension ref="A1:C80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
       <c r="C1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B17" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B19" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" t="s">
+        <v>348</v>
+      </c>
+      <c r="C33" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" t="s">
+        <v>348</v>
+      </c>
+      <c r="C35" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" t="s">
+        <v>348</v>
+      </c>
+      <c r="C37" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>350</v>
+      </c>
+      <c r="C38" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B41" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B45" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B46" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B51" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B53" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B57" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" t="s">
+        <v>348</v>
+      </c>
+      <c r="C58" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" t="s">
+        <v>350</v>
+      </c>
+      <c r="C59" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B61" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B66" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B69" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B70" t="s">
+        <v>350</v>
+      </c>
+      <c r="C70" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B71" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B72" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B74" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B75" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B77" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B79" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B80" xr:uid="{E95FDA58-DA1C-47A2-B6D3-A13747077D0C}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85AFABB-8C66-4072-B321-253033877C51}">
+  <dimension ref="A1:C84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="B5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B24" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B29" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B34" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B39" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B40" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B41" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B45" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B46" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B47" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B48" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B49" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B50" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B53" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B54" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B55" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B56" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B57" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B60" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B62" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B63" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B64" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B66" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B68" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B69" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B70" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B71" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B72" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B73" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B74" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B75" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B76" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B77" t="s">
+        <v>328</v>
+      </c>
+      <c r="C77" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B78" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B79" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B80" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B81" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B82" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5045D7-697C-4873-B3E1-99950E815A7E}">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C9" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
+      <c r="C11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
+      <c r="A17" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>58</v>
+      <c r="A18" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B18" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>89</v>
+      <c r="A19" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>88</v>
+      <c r="A20" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B23" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C28" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B29" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>328</v>
+      </c>
+      <c r="C30" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C32" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B33" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C34" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8986A61A-6FFC-4A57-8CD4-3DC9C8CB7DC8}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="B13" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B17" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B19" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B20" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>7</v>
+      <c r="B21" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E56">
-    <sortCondition ref="B2:B56"/>
-    <sortCondition ref="A2:A56"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
analyze GEOME metadata fields, summary in this file
</commit_message>
<xml_diff>
--- a/examples/GEOME/requiredFieldsWork.xlsx
+++ b/examples/GEOME/requiredFieldsWork.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\examples\GEOME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF473A0-9BD8-45D5-9B97-440F3029A28D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244E4CFA-CCAD-431C-95A1-B72D62ACF682}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="1725" windowWidth="15195" windowHeight="14250" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1305" windowWidth="15195" windowHeight="14250" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summaryStart" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EventColumns!$B$1:$B$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">summaryStart!$A$1:$D$1870</definedName>
+    <definedName name="column_name">'All required columns'!$A$2:$A$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
     <author>Stephen Richard</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{ED1E6B16-6ACB-4692-B8D3-6604EA396846}">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{ED1E6B16-6ACB-4692-B8D3-6604EA396846}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{43A738C5-2997-498B-8A50-B9C59B9638C4}">
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{43A738C5-2997-498B-8A50-B9C59B9638C4}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{2FFDF1BE-1A72-4B03-B76C-175F8FD4D905}">
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{2FFDF1BE-1A72-4B03-B76C-175F8FD4D905}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{17497B20-C224-45EB-BF10-847B83285A1F}">
+    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{17497B20-C224-45EB-BF10-847B83285A1F}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{DD1DFC0E-B7AE-48DF-9130-EEF04611D7FF}">
+    <comment ref="A40" authorId="0" shapeId="0" xr:uid="{DD1DFC0E-B7AE-48DF-9130-EEF04611D7FF}">
       <text>
         <r>
           <rPr>
@@ -113,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{E2C0BAD5-140C-4ABC-8682-609C4D3244C6}">
+    <comment ref="A42" authorId="0" shapeId="0" xr:uid="{E2C0BAD5-140C-4ABC-8682-609C4D3244C6}">
       <text>
         <r>
           <rPr>
@@ -126,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{FF882C6F-99CA-4786-89BE-3CB7E9BA9A3A}">
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{FF882C6F-99CA-4786-89BE-3CB7E9BA9A3A}">
       <text>
         <r>
           <rPr>
@@ -139,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A49" authorId="0" shapeId="0" xr:uid="{C841E628-2BBE-46FE-AC35-4E82A892C133}">
+    <comment ref="A54" authorId="0" shapeId="0" xr:uid="{C841E628-2BBE-46FE-AC35-4E82A892C133}">
       <text>
         <r>
           <rPr>
@@ -152,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{69D861B2-8665-494E-AE7E-360F1A8A5048}">
+    <comment ref="A73" authorId="0" shapeId="0" xr:uid="{69D861B2-8665-494E-AE7E-360F1A8A5048}">
       <text>
         <r>
           <rPr>
@@ -165,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A71" authorId="0" shapeId="0" xr:uid="{17B7DB97-1F4E-4CCC-9E00-1D584BA79657}">
+    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{17B7DB97-1F4E-4CCC-9E00-1D584BA79657}">
       <text>
         <r>
           <rPr>
@@ -188,7 +189,33 @@
     <author>Stephen Richard</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5BD01C06-4ACF-42DD-A3B7-8544BD8664AB}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{4EC38C09-97AC-4CD3-A8D3-BE5213930422}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The specific nature of the data record.  Examples include PreservedSpecimen, FossilSpecimen, LivingSpecimen, MaterialSample, Event, HumanObservation, MachineObservation, Taxon, Occurrence</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{02B0006C-EF28-409F-ACF0-9738C8706E3A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The name (or acronym) in use by the institution having custody of the object(s) or information referred to in the record.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{5BD01C06-4ACF-42DD-A3B7-8544BD8664AB}">
       <text>
         <r>
           <rPr>
@@ -201,20 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{4EC38C09-97AC-4CD3-A8D3-BE5213930422}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The specific nature of the data record.  Examples include PreservedSpecimen, FossilSpecimen, LivingSpecimen, MaterialSample, Event, HumanObservation, MachineObservation, Taxon, Occurrence</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{A292817E-A316-4EC6-B325-D832CEEE9F8F}">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{A292817E-A316-4EC6-B325-D832CEEE9F8F}">
       <text>
         <r>
           <rPr>
@@ -227,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{1E4F74CB-EE8F-4BA2-B2D7-F464ED1A2A06}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{1E4F74CB-EE8F-4BA2-B2D7-F464ED1A2A06}">
       <text>
         <r>
           <rPr>
@@ -240,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{0208210E-5787-4662-8D5D-AB1D8852A7B9}">
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{0208210E-5787-4662-8D5D-AB1D8852A7B9}">
       <text>
         <r>
           <rPr>
@@ -253,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{C458E9D0-67F5-4411-A2E9-019F0F18C2FB}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{C458E9D0-67F5-4411-A2E9-019F0F18C2FB}">
       <text>
         <r>
           <rPr>
@@ -266,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{A22EB3D2-1C22-4F1B-A26D-AEECD0DF2969}">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{A22EB3D2-1C22-4F1B-A26D-AEECD0DF2969}">
       <text>
         <r>
           <rPr>
@@ -279,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{02CACFDA-04D9-4356-8705-31F01130480C}">
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{02CACFDA-04D9-4356-8705-31F01130480C}">
       <text>
         <r>
           <rPr>
@@ -292,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{E6D03C7F-F924-4CE2-B8A0-27D99087260C}">
+    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{E6D03C7F-F924-4CE2-B8A0-27D99087260C}">
       <text>
         <r>
           <rPr>
@@ -305,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{F22EAB9C-E145-4DDA-983D-3C71A7792B9C}">
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{F22EAB9C-E145-4DDA-983D-3C71A7792B9C}">
       <text>
         <r>
           <rPr>
@@ -318,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{1A9ED1DC-B056-4B4B-B65E-117093C0D1A4}">
+    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{1A9ED1DC-B056-4B4B-B65E-117093C0D1A4}">
       <text>
         <r>
           <rPr>
@@ -331,20 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{02B0006C-EF28-409F-ACF0-9738C8706E3A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The name (or acronym) in use by the institution having custody of the object(s) or information referred to in the record.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{02694076-D448-4E4A-A2AF-E1A3B62A0E44}">
+    <comment ref="A46" authorId="0" shapeId="0" xr:uid="{02694076-D448-4E4A-A2AF-E1A3B62A0E44}">
       <text>
         <r>
           <rPr>
@@ -357,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A42" authorId="0" shapeId="0" xr:uid="{88E249DA-588C-416B-A4E6-96B9455A39CB}">
+    <comment ref="A47" authorId="0" shapeId="0" xr:uid="{88E249DA-588C-416B-A4E6-96B9455A39CB}">
       <text>
         <r>
           <rPr>
@@ -370,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{62760569-B8D9-4E62-B61C-79C12AAC91B7}">
+    <comment ref="A48" authorId="0" shapeId="0" xr:uid="{62760569-B8D9-4E62-B61C-79C12AAC91B7}">
       <text>
         <r>
           <rPr>
@@ -383,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A47" authorId="0" shapeId="0" xr:uid="{D41A34C7-01B7-42D7-9760-AA4714054934}">
+    <comment ref="A52" authorId="0" shapeId="0" xr:uid="{D41A34C7-01B7-42D7-9760-AA4714054934}">
       <text>
         <r>
           <rPr>
@@ -396,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{C868859C-E2AE-47B9-93A3-1EE01516C63F}">
+    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{C868859C-E2AE-47B9-93A3-1EE01516C63F}">
       <text>
         <r>
           <rPr>
@@ -432,7 +433,7 @@
     <author>Stephen Richard</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{AC4C5A15-9190-46C3-B980-EC392FDA3E14}">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{AC4C5A15-9190-46C3-B980-EC392FDA3E14}">
       <text>
         <r>
           <rPr>
@@ -450,7 +451,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6109" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6117" uniqueCount="373">
   <si>
     <t>record_alias</t>
   </si>
@@ -1445,18 +1446,12 @@
     <t>context</t>
   </si>
   <si>
-    <t>samplingEvent.responsibleParty</t>
-  </si>
-  <si>
     <t>samplingSite.placeName</t>
   </si>
   <si>
     <t>GeospatialLocation.positionUncertainty</t>
   </si>
   <si>
-    <t>GeospatialDDCoordLocation</t>
-  </si>
-  <si>
     <t>GeospatialLocation.</t>
   </si>
   <si>
@@ -1551,13 +1546,37 @@
   </si>
   <si>
     <t>related to measurement, not sample</t>
+  </si>
+  <si>
+    <t>samplingSite.keyword</t>
+  </si>
+  <si>
+    <t>SamplingEvent.@id</t>
+  </si>
+  <si>
+    <t>bcid</t>
+  </si>
+  <si>
+    <t>metadata record @id</t>
+  </si>
+  <si>
+    <t>metadata:' &amp; sample.bcid</t>
+  </si>
+  <si>
+    <t>requiredSomewhere</t>
+  </si>
+  <si>
+    <t>GeospatialDDCoordLocation.latitude</t>
+  </si>
+  <si>
+    <t>GeospatialDDCoordLocation.longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1697,6 +1716,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1996,7 +2023,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2039,8 +2066,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2051,8 +2079,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2086,6 +2117,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2096,7 +2128,57 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -28601,7 +28683,7 @@
   <dimension ref="A1:A47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection sqref="A1:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28609,12 +28691,12 @@
     <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -28851,708 +28933,1065 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A472B710-19EE-4903-8EC9-3BCEC24609CC}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" t="b">
+        <f>IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" t="b">
+        <f>IF(ISERROR(VLOOKUP(A3,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" t="b">
+        <f>IF(ISERROR(VLOOKUP(A4,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5" t="b">
+        <f>IF(ISERROR(VLOOKUP(A5,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D6" t="b">
+        <f>IF(ISERROR(VLOOKUP(A6,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" t="b">
+        <f>IF(ISERROR(VLOOKUP(A7,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" t="b">
+        <f>IF(ISERROR(VLOOKUP(A8,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" t="b">
+        <f>IF(ISERROR(VLOOKUP(A9,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" t="s">
+        <v>337</v>
+      </c>
+      <c r="D10" t="b">
+        <f>IF(ISERROR(VLOOKUP(A10,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="D11" t="b">
+        <f>IF(ISERROR(VLOOKUP(A11,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>336</v>
+      </c>
+      <c r="D12" t="b">
+        <f>IF(ISERROR(VLOOKUP(A12,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>340</v>
+      </c>
+      <c r="D13" t="b">
+        <f>IF(ISERROR(VLOOKUP(A13,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" t="b">
+        <f>IF(ISERROR(VLOOKUP(A14,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D15" t="b">
+        <f>IF(ISERROR(VLOOKUP(A15,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
         <v>346</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C16" t="s">
+        <v>337</v>
+      </c>
+      <c r="D16" t="b">
+        <f>IF(ISERROR(VLOOKUP(A16,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D17" t="b">
+        <f>IF(ISERROR(VLOOKUP(A17,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B4" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B18" t="s">
+        <v>345</v>
+      </c>
+      <c r="D18" t="b">
+        <f>IF(ISERROR(VLOOKUP(A18,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B19" t="s">
+        <v>345</v>
+      </c>
+      <c r="D19" t="b">
+        <f>IF(ISERROR(VLOOKUP(A19,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B6" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B20" t="s">
+        <v>345</v>
+      </c>
+      <c r="D20" t="b">
+        <f>IF(ISERROR(VLOOKUP(A20,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D21" t="b">
+        <f>IF(ISERROR(VLOOKUP(A21,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="D22" t="b">
+        <f>IF(ISERROR(VLOOKUP(A22,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B23" t="s">
+        <v>331</v>
+      </c>
+      <c r="D23" t="b">
+        <f>IF(ISERROR(VLOOKUP(A23,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B13" t="s">
-        <v>349</v>
-      </c>
-      <c r="C13" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" t="s">
-        <v>349</v>
-      </c>
-      <c r="C14" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B19" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B22" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B23" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="B24" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>337</v>
+      </c>
+      <c r="D24" t="b">
+        <f>IF(ISERROR(VLOOKUP(A24,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>337</v>
+      </c>
+      <c r="D25" t="b">
+        <f>IF(ISERROR(VLOOKUP(A25,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B26" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="b">
+        <f>IF(ISERROR(VLOOKUP(A26,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="b">
+        <f>IF(ISERROR(VLOOKUP(A27,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>327</v>
+      </c>
+      <c r="D28" t="b">
+        <f>IF(ISERROR(VLOOKUP(A28,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s">
+        <v>333</v>
+      </c>
+      <c r="D29" t="b">
+        <f>IF(ISERROR(VLOOKUP(A29,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" t="s">
+        <v>334</v>
+      </c>
+      <c r="D30" t="b">
+        <f>IF(ISERROR(VLOOKUP(A30,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" t="s">
+        <v>335</v>
+      </c>
+      <c r="D31" t="b">
+        <f>IF(ISERROR(VLOOKUP(A31,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" t="s">
+        <v>345</v>
+      </c>
+      <c r="D32" t="b">
+        <f>IF(ISERROR(VLOOKUP(A32,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" t="s">
+        <v>345</v>
+      </c>
+      <c r="D33" t="b">
+        <f>IF(ISERROR(VLOOKUP(A33,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" t="s">
+        <v>345</v>
+      </c>
+      <c r="D34" t="b">
+        <f>IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" t="s">
+        <v>345</v>
+      </c>
+      <c r="D35" t="b">
+        <f>IF(ISERROR(VLOOKUP(A35,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
+        <v>345</v>
+      </c>
+      <c r="D36" t="b">
+        <f>IF(ISERROR(VLOOKUP(A36,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="B28" t="s">
-        <v>350</v>
-      </c>
-      <c r="C28" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B33" t="s">
-        <v>348</v>
-      </c>
-      <c r="C33" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B34" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35" t="s">
-        <v>348</v>
-      </c>
-      <c r="C35" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="B37" t="s">
         <v>348</v>
       </c>
       <c r="C37" t="s">
+        <v>337</v>
+      </c>
+      <c r="D37" t="b">
+        <f>IF(ISERROR(VLOOKUP(A37,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" t="s">
+        <v>326</v>
+      </c>
+      <c r="D38" t="b">
+        <f>IF(ISERROR(VLOOKUP(A38,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" t="s">
+        <v>326</v>
+      </c>
+      <c r="D39" t="b">
+        <f>IF(ISERROR(VLOOKUP(A39,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" t="s">
+        <v>346</v>
+      </c>
+      <c r="C40" t="s">
+        <v>337</v>
+      </c>
+      <c r="D40" t="b">
+        <f>IF(ISERROR(VLOOKUP(A40,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" t="s">
+        <v>336</v>
+      </c>
+      <c r="D41" t="b">
+        <f>IF(ISERROR(VLOOKUP(A41,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" t="s">
+        <v>346</v>
+      </c>
+      <c r="C42" t="s">
+        <v>337</v>
+      </c>
+      <c r="D42" t="b">
+        <f>IF(ISERROR(VLOOKUP(A42,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" t="s">
+        <v>346</v>
+      </c>
+      <c r="C43" t="s">
+        <v>337</v>
+      </c>
+      <c r="D43" t="b">
+        <f>IF(ISERROR(VLOOKUP(A43,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>346</v>
+      </c>
+      <c r="D44" t="b">
+        <f>IF(ISERROR(VLOOKUP(A44,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" t="s">
+        <v>334</v>
+      </c>
+      <c r="D45" t="b">
+        <f>IF(ISERROR(VLOOKUP(A45,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" t="s">
+        <v>365</v>
+      </c>
+      <c r="D46" t="b">
+        <f>IF(ISERROR(VLOOKUP(A46,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" t="s">
+        <v>365</v>
+      </c>
+      <c r="D47" t="b">
+        <f>IF(ISERROR(VLOOKUP(A47,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" t="s">
+        <v>329</v>
+      </c>
+      <c r="D48" t="b">
+        <f>IF(ISERROR(VLOOKUP(A48,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" t="s">
+        <v>345</v>
+      </c>
+      <c r="D49" t="b">
+        <f>IF(ISERROR(VLOOKUP(A49,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" t="s">
+        <v>345</v>
+      </c>
+      <c r="D50" t="b">
+        <f>IF(ISERROR(VLOOKUP(A50,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" t="s">
+        <v>345</v>
+      </c>
+      <c r="D51" t="b">
+        <f>IF(ISERROR(VLOOKUP(A51,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" t="s">
+        <v>345</v>
+      </c>
+      <c r="D52" t="b">
+        <f>IF(ISERROR(VLOOKUP(A52,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" t="s">
+        <v>345</v>
+      </c>
+      <c r="D53" t="b">
+        <f>IF(ISERROR(VLOOKUP(A53,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" t="s">
+        <v>346</v>
+      </c>
+      <c r="D54" t="b">
+        <f>IF(ISERROR(VLOOKUP(A54,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" t="s">
+        <v>338</v>
+      </c>
+      <c r="D55" t="b">
+        <f>IF(ISERROR(VLOOKUP(A55,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B56" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" t="s">
-        <v>350</v>
-      </c>
-      <c r="C38" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D56" t="b">
+        <f>IF(ISERROR(VLOOKUP(A56,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" t="s">
+        <v>346</v>
+      </c>
+      <c r="D57" t="b">
+        <f>IF(ISERROR(VLOOKUP(A57,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" t="s">
+        <v>345</v>
+      </c>
+      <c r="D58" t="b">
+        <f>IF(ISERROR(VLOOKUP(A58,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" t="s">
+        <v>345</v>
+      </c>
+      <c r="D59" t="b">
+        <f>IF(ISERROR(VLOOKUP(A59,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B60" t="s">
+        <v>335</v>
+      </c>
+      <c r="D60" t="b">
+        <f>IF(ISERROR(VLOOKUP(A60,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" t="s">
+        <v>335</v>
+      </c>
+      <c r="D61" t="b">
+        <f>IF(ISERROR(VLOOKUP(A61,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" t="s">
+        <v>346</v>
+      </c>
+      <c r="C62" t="s">
+        <v>337</v>
+      </c>
+      <c r="D62" t="b">
+        <f>IF(ISERROR(VLOOKUP(A62,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D63" t="b">
+        <f>IF(ISERROR(VLOOKUP(A63,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B41" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B42" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C64" t="s">
+        <v>337</v>
+      </c>
+      <c r="D64" t="b">
+        <f>IF(ISERROR(VLOOKUP(A64,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B65" t="s">
+        <v>345</v>
+      </c>
+      <c r="D65" t="b">
+        <f>IF(ISERROR(VLOOKUP(A65,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" t="s">
+        <v>345</v>
+      </c>
+      <c r="D66" t="b">
+        <f>IF(ISERROR(VLOOKUP(A66,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" t="s">
+        <v>335</v>
+      </c>
+      <c r="D67" t="b">
+        <f>IF(ISERROR(VLOOKUP(A67,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" t="s">
+        <v>335</v>
+      </c>
+      <c r="D68" t="b">
+        <f>IF(ISERROR(VLOOKUP(A68,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" t="s">
+        <v>327</v>
+      </c>
+      <c r="D69" t="b">
+        <f>IF(ISERROR(VLOOKUP(A69,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" t="s">
+        <v>331</v>
+      </c>
+      <c r="D70" t="b">
+        <f>IF(ISERROR(VLOOKUP(A70,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B44" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B45" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B46" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B47" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B48" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="D71" t="b">
+        <f>IF(ISERROR(VLOOKUP(A71,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B72" t="s">
+        <v>365</v>
+      </c>
+      <c r="D72" t="b">
+        <f>IF(ISERROR(VLOOKUP(A72,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B73" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C73" t="s">
+        <v>337</v>
+      </c>
+      <c r="D73" t="b">
+        <f>IF(ISERROR(VLOOKUP(A73,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B74" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B53" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B54" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B55" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B56" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B57" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" t="s">
-        <v>348</v>
-      </c>
-      <c r="C58" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B59" t="s">
-        <v>350</v>
-      </c>
-      <c r="C59" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B60" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B61" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B62" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B63" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B64" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B65" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B66" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B67" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B68" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B69" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B70" t="s">
-        <v>350</v>
-      </c>
-      <c r="C70" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B71" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="D74" t="b">
+        <f>IF(ISERROR(VLOOKUP(A74,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B72" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B73" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B74" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="B75" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="b">
+        <f>IF(ISERROR(VLOOKUP(A75,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B76" t="s">
+        <v>335</v>
+      </c>
+      <c r="D76" t="b">
+        <f>IF(ISERROR(VLOOKUP(A76,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B77" t="s">
+        <v>335</v>
+      </c>
+      <c r="D77" t="b">
+        <f>IF(ISERROR(VLOOKUP(A77,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B78" t="s">
+        <v>327</v>
+      </c>
+      <c r="D78" t="b">
+        <f>IF(ISERROR(VLOOKUP(A78,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B76" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="B79" t="s">
+        <v>334</v>
+      </c>
+      <c r="D79" t="b">
+        <f>IF(ISERROR(VLOOKUP(A79,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B77" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="B80" t="s">
+        <v>331</v>
+      </c>
+      <c r="D80" t="b">
+        <f>IF(ISERROR(VLOOKUP(A80,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B78" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="B81" t="s">
+        <v>334</v>
+      </c>
+      <c r="D81" t="b">
+        <f>IF(ISERROR(VLOOKUP(A81,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B79" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B80" t="s">
-        <v>327</v>
+      <c r="B82" t="s">
+        <v>331</v>
+      </c>
+      <c r="D82" t="b">
+        <f>IF(ISERROR(VLOOKUP(A82,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:B80" xr:uid="{E95FDA58-DA1C-47A2-B6D3-A13747077D0C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D82">
+    <sortCondition descending="1" ref="D2:D82"/>
+    <sortCondition ref="A2:A82"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:A82">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>D2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{B774F272-58C3-4C7F-ABD6-4D9D2E625017}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{FEBCC76C-7882-489D-BBCC-8B7CC5377C3E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85AFABB-8C66-4072-B321-253033877C51}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29561,612 +30000,915 @@
     <col min="2" max="2" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
-        <v>346</v>
-      </c>
       <c r="C1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="D1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" t="b">
+        <f>IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" t="b">
+        <f>IF(ISERROR(VLOOKUP(A3,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>352</v>
+      </c>
+      <c r="D4" t="b">
+        <f>IF(ISERROR(VLOOKUP(A4,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D5" t="b">
+        <f>IF(ISERROR(VLOOKUP(A5,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" t="b">
+        <f>IF(ISERROR(VLOOKUP(A6,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="b">
+        <f>IF(ISERROR(VLOOKUP(A7,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>352</v>
+      </c>
+      <c r="D8" t="b">
+        <f>IF(ISERROR(VLOOKUP(A8,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" t="b">
+        <f>IF(ISERROR(VLOOKUP(A9,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>352</v>
+      </c>
+      <c r="D10" t="b">
+        <f>IF(ISERROR(VLOOKUP(A10,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D11" t="b">
+        <f>IF(ISERROR(VLOOKUP(A11,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" t="s">
+        <v>357</v>
+      </c>
+      <c r="D12" t="b">
+        <f>IF(ISERROR(VLOOKUP(A12,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B13" t="s">
+        <v>349</v>
+      </c>
+      <c r="D13" t="b">
+        <f>IF(ISERROR(VLOOKUP(A13,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B14" t="s">
+        <v>349</v>
+      </c>
+      <c r="D14" t="b">
+        <f>IF(ISERROR(VLOOKUP(A14,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B4" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D15" t="b">
+        <f>IF(ISERROR(VLOOKUP(A15,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B16" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="D16" t="b">
+        <f>IF(ISERROR(VLOOKUP(A16,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="B7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B12" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B13" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B14" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B16" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="B17" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" t="b">
+        <f>IF(ISERROR(VLOOKUP(A17,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D18" t="b">
+        <f>IF(ISERROR(VLOOKUP(A18,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" t="s">
+        <v>351</v>
+      </c>
+      <c r="D19" t="b">
+        <f>IF(ISERROR(VLOOKUP(A19,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B20" t="s">
+        <v>353</v>
+      </c>
+      <c r="D20" t="b">
+        <f>IF(ISERROR(VLOOKUP(A20,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D21" t="b">
+        <f>IF(ISERROR(VLOOKUP(A21,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s">
+        <v>354</v>
+      </c>
+      <c r="D22" t="b">
+        <f>IF(ISERROR(VLOOKUP(A22,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" t="s">
+        <v>355</v>
+      </c>
+      <c r="D23" t="b">
+        <f>IF(ISERROR(VLOOKUP(A23,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" t="s">
+        <v>330</v>
+      </c>
+      <c r="D24" t="b">
+        <f>IF(ISERROR(VLOOKUP(A24,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" t="s">
+        <v>352</v>
+      </c>
+      <c r="D25" t="b">
+        <f>IF(ISERROR(VLOOKUP(A25,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" t="s">
+        <v>322</v>
+      </c>
+      <c r="D26" t="b">
+        <f>IF(ISERROR(VLOOKUP(A26,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B27" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="D27" t="b">
+        <f>IF(ISERROR(VLOOKUP(A27,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D28" t="b">
+        <f>IF(ISERROR(VLOOKUP(A28,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" t="b">
+        <f>IF(ISERROR(VLOOKUP(A29,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B30" t="s">
+        <v>326</v>
+      </c>
+      <c r="D30" t="b">
+        <f>IF(ISERROR(VLOOKUP(A30,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" t="s">
+        <v>355</v>
+      </c>
+      <c r="D31" t="b">
+        <f>IF(ISERROR(VLOOKUP(A31,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" t="s">
+        <v>355</v>
+      </c>
+      <c r="D32" t="b">
+        <f>IF(ISERROR(VLOOKUP(A32,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B33" t="s">
+        <v>349</v>
+      </c>
+      <c r="D33" t="b">
+        <f>IF(ISERROR(VLOOKUP(A33,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B34" t="s">
+        <v>329</v>
+      </c>
+      <c r="D34" t="b">
+        <f>IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35" t="s">
+        <v>352</v>
+      </c>
+      <c r="D35" t="b">
+        <f>IF(ISERROR(VLOOKUP(A35,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" t="s">
+        <v>352</v>
+      </c>
+      <c r="D36" t="b">
+        <f>IF(ISERROR(VLOOKUP(A36,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B37" t="s">
+        <v>352</v>
+      </c>
+      <c r="D37" t="b">
+        <f>IF(ISERROR(VLOOKUP(A37,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B38" t="s">
+        <v>323</v>
+      </c>
+      <c r="D38" t="b">
+        <f>IF(ISERROR(VLOOKUP(A38,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B39" t="s">
+        <v>355</v>
+      </c>
+      <c r="D39" t="b">
+        <f>IF(ISERROR(VLOOKUP(A39,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" t="s">
+        <v>355</v>
+      </c>
+      <c r="D40" t="b">
+        <f>IF(ISERROR(VLOOKUP(A40,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" t="s">
+        <v>328</v>
+      </c>
+      <c r="D41" t="b">
+        <f>IF(ISERROR(VLOOKUP(A41,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B42" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B21" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B22" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B23" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B24" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B25" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B26" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B27" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B28" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B29" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B31" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B33" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B34" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B35" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B37" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="D42" t="b">
+        <f>IF(ISERROR(VLOOKUP(A42,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="B38" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B39" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B40" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B41" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="B43" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D43" t="b">
+        <f>IF(ISERROR(VLOOKUP(A43,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+      <c r="D44" t="b">
+        <f>IF(ISERROR(VLOOKUP(A44,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B45" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D45" t="b">
+        <f>IF(ISERROR(VLOOKUP(A45,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B46" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+      <c r="D46" t="b">
+        <f>IF(ISERROR(VLOOKUP(A46,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B47" t="s">
+        <v>353</v>
+      </c>
+      <c r="D47" t="b">
+        <f>IF(ISERROR(VLOOKUP(A47,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" t="s">
+        <v>352</v>
+      </c>
+      <c r="D48" t="b">
+        <f>IF(ISERROR(VLOOKUP(A48,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B49" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B48" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B49" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D49" t="b">
+        <f>IF(ISERROR(VLOOKUP(A49,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B50" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50" t="b">
+        <f>IF(ISERROR(VLOOKUP(A50,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B51" t="s">
+        <v>352</v>
+      </c>
+      <c r="D51" t="b">
+        <f>IF(ISERROR(VLOOKUP(A51,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B52" t="s">
+        <v>322</v>
+      </c>
+      <c r="D52" t="b">
+        <f>IF(ISERROR(VLOOKUP(A52,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B53" t="s">
+        <v>355</v>
+      </c>
+      <c r="D53" t="b">
+        <f>IF(ISERROR(VLOOKUP(A53,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B54" t="s">
+        <v>355</v>
+      </c>
+      <c r="D54" t="b">
+        <f>IF(ISERROR(VLOOKUP(A54,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B55" t="s">
+        <v>326</v>
+      </c>
+      <c r="D55" t="b">
+        <f>IF(ISERROR(VLOOKUP(A55,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B56" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="D56" t="b">
+        <f>IF(ISERROR(VLOOKUP(A56,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="B53" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B54" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B55" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B56" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="B57" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D57" t="b">
+        <f>IF(ISERROR(VLOOKUP(A57,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>31</v>
+        <v>253</v>
       </c>
       <c r="B58" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+      <c r="D58" t="b">
+        <f>IF(ISERROR(VLOOKUP(A58,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>40</v>
+        <v>254</v>
       </c>
       <c r="B59" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="D59" t="b">
+        <f>IF(ISERROR(VLOOKUP(A59,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B60" t="s">
+        <v>349</v>
+      </c>
+      <c r="D60" t="b">
+        <f>IF(ISERROR(VLOOKUP(A60,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B61" t="s">
+        <v>323</v>
+      </c>
+      <c r="D61" t="b">
+        <f>IF(ISERROR(VLOOKUP(A61,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B60" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="B62" t="s">
+        <v>355</v>
+      </c>
+      <c r="D62" t="b">
+        <f>IF(ISERROR(VLOOKUP(A62,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B62" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="B63" t="s">
+        <v>352</v>
+      </c>
+      <c r="D63" t="b">
+        <f>IF(ISERROR(VLOOKUP(A63,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B63" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="B64" t="s">
+        <v>352</v>
+      </c>
+      <c r="D64" t="b">
+        <f>IF(ISERROR(VLOOKUP(A64,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B64" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="B65" t="s">
+        <v>352</v>
+      </c>
+      <c r="D65" t="b">
+        <f>IF(ISERROR(VLOOKUP(A65,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B65" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="B66" t="s">
+        <v>352</v>
+      </c>
+      <c r="D66" t="b">
+        <f>IF(ISERROR(VLOOKUP(A66,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B66" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="B67" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D67" t="b">
+        <f>IF(ISERROR(VLOOKUP(A67,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>263</v>
       </c>
       <c r="B68" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+      <c r="D68" t="b">
+        <f>IF(ISERROR(VLOOKUP(A68,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>264</v>
       </c>
       <c r="B69" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D69" t="b">
+        <f>IF(ISERROR(VLOOKUP(A69,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>265</v>
       </c>
       <c r="B70" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D70" t="b">
+        <f>IF(ISERROR(VLOOKUP(A70,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>266</v>
       </c>
       <c r="B71" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D71" t="b">
+        <f>IF(ISERROR(VLOOKUP(A71,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>267</v>
       </c>
       <c r="B72" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D72" t="b">
+        <f>IF(ISERROR(VLOOKUP(A72,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>268</v>
       </c>
       <c r="B73" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D73" t="b">
+        <f>IF(ISERROR(VLOOKUP(A73,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B74" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="b">
+        <f>IF(ISERROR(VLOOKUP(A74,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>270</v>
       </c>
       <c r="B75" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="b">
+        <f>IF(ISERROR(VLOOKUP(A75,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B76" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="D76" t="b">
+        <f>IF(ISERROR(VLOOKUP(A76,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>272</v>
       </c>
@@ -30174,66 +30916,107 @@
         <v>328</v>
       </c>
       <c r="C77" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="D77" t="b">
+        <f>IF(ISERROR(VLOOKUP(A77,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B78" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="b">
+        <f>IF(ISERROR(VLOOKUP(A78,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B79" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="b">
+        <f>IF(ISERROR(VLOOKUP(A79,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>275</v>
       </c>
       <c r="B80" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D80" t="b">
+        <f>IF(ISERROR(VLOOKUP(A80,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>276</v>
       </c>
       <c r="B81" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="D81" t="b">
+        <f>IF(ISERROR(VLOOKUP(A81,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>277</v>
       </c>
       <c r="B82" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="D82" t="b">
+        <f>IF(ISERROR(VLOOKUP(A82,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>278</v>
       </c>
       <c r="B83" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D83" t="b">
+        <f>IF(ISERROR(VLOOKUP(A83,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B84" t="s">
-        <v>356</v>
+        <v>354</v>
+      </c>
+      <c r="D84" t="b">
+        <f>IF(ISERROR(VLOOKUP(A84,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
+    <sortCondition descending="1" ref="D2:D84"/>
+    <sortCondition ref="A2:A84"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:A84">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>D2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -30241,310 +31024,459 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5045D7-697C-4873-B3E1-99950E815A7E}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
-        <v>346</v>
-      </c>
       <c r="C1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="D1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" t="b">
+        <f>IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>364</v>
+      </c>
+      <c r="D3" t="b">
+        <f>IF(ISERROR(VLOOKUP(A3,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" t="b">
+        <f>IF(ISERROR(VLOOKUP(A4,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>364</v>
+      </c>
+      <c r="D5" t="b">
+        <f>IF(ISERROR(VLOOKUP(A5,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D6" t="b">
+        <f>IF(ISERROR(VLOOKUP(A6,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D7" t="b">
+        <f>IF(ISERROR(VLOOKUP(A7,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" t="b">
+        <f>IF(ISERROR(VLOOKUP(A8,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>362</v>
+      </c>
+      <c r="D9" t="b">
+        <f>IF(ISERROR(VLOOKUP(A9,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" t="b">
+        <f>IF(ISERROR(VLOOKUP(A10,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>328</v>
+      </c>
+      <c r="C11" t="s">
+        <v>363</v>
+      </c>
+      <c r="D11" t="b">
+        <f>IF(ISERROR(VLOOKUP(A11,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" t="b">
+        <f>IF(ISERROR(VLOOKUP(A12,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D13" t="b">
+        <f>IF(ISERROR(VLOOKUP(A13,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B14" t="s">
+        <v>359</v>
+      </c>
+      <c r="D14" t="b">
+        <f>IF(ISERROR(VLOOKUP(A14,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C15" t="s">
+        <v>364</v>
+      </c>
+      <c r="D15" t="b">
+        <f>IF(ISERROR(VLOOKUP(A15,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C16" t="s">
+        <v>364</v>
+      </c>
+      <c r="D16" t="b">
+        <f>IF(ISERROR(VLOOKUP(A16,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" t="s">
+        <v>364</v>
+      </c>
+      <c r="D17" t="b">
+        <f>IF(ISERROR(VLOOKUP(A17,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" t="s">
+        <v>364</v>
+      </c>
+      <c r="D18" t="b">
+        <f>IF(ISERROR(VLOOKUP(A18,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" t="s">
+        <v>364</v>
+      </c>
+      <c r="D19" t="b">
+        <f>IF(ISERROR(VLOOKUP(A19,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" t="b">
+        <f>IF(ISERROR(VLOOKUP(A20,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B21" t="s">
+        <v>355</v>
+      </c>
+      <c r="D21" t="b">
+        <f>IF(ISERROR(VLOOKUP(A21,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C22" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B4" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C5" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="C8" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C12" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C14" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="B15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D22" t="b">
+        <f>IF(ISERROR(VLOOKUP(A22,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B23" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B17" t="s">
-        <v>363</v>
-      </c>
-      <c r="C17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D23" t="b">
+        <f>IF(ISERROR(VLOOKUP(A23,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" t="s">
+        <v>362</v>
+      </c>
+      <c r="D24" t="b">
+        <f>IF(ISERROR(VLOOKUP(A24,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B25" t="s">
+        <v>362</v>
+      </c>
+      <c r="D25" t="b">
+        <f>IF(ISERROR(VLOOKUP(A25,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B26" t="s">
+        <v>362</v>
+      </c>
+      <c r="D26" t="b">
+        <f>IF(ISERROR(VLOOKUP(A26,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27" t="s">
+        <v>362</v>
+      </c>
+      <c r="D27" t="b">
+        <f>IF(ISERROR(VLOOKUP(A27,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B28" t="s">
+        <v>362</v>
+      </c>
+      <c r="D28" t="b">
+        <f>IF(ISERROR(VLOOKUP(A28,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C29" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B19" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="B20" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B22" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="B23" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B24" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C28" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="D29" t="b">
+        <f>IF(ISERROR(VLOOKUP(A29,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B29" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="B30" t="s">
-        <v>328</v>
-      </c>
-      <c r="C30" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+      <c r="D30" t="b">
+        <f>IF(ISERROR(VLOOKUP(A30,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>299</v>
       </c>
       <c r="B31" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="b">
+        <f>IF(ISERROR(VLOOKUP(A31,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>300</v>
       </c>
       <c r="C32" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+      <c r="D32" t="b">
+        <f>IF(ISERROR(VLOOKUP(A32,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>301</v>
       </c>
       <c r="B33" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="D33" t="b">
+        <f>IF(ISERROR(VLOOKUP(A33,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>302</v>
       </c>
       <c r="C34" t="s">
-        <v>366</v>
+        <v>364</v>
+      </c>
+      <c r="D34" t="b">
+        <f>IF(ISERROR(VLOOKUP(A34,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D34">
+    <sortCondition descending="1" ref="D2:D34"/>
+    <sortCondition ref="A2:A34"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:A34">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>D1048546</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>D2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8986A61A-6FFC-4A57-8CD4-3DC9C8CB7DC8}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30553,178 +31485,270 @@
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
-        <v>346</v>
-      </c>
       <c r="C1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="D1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" t="b">
+        <f>IF(ISERROR(VLOOKUP(A2,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="b">
+        <f>IF(ISERROR(VLOOKUP(A3,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D4" t="b">
+        <f>IF(ISERROR(VLOOKUP(A4,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" t="b">
+        <f>IF(ISERROR(VLOOKUP(A5,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D6" t="b">
+        <f>IF(ISERROR(VLOOKUP(A6,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="D7" t="b">
+        <f>IF(ISERROR(VLOOKUP(A7,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="D8" t="b">
+        <f>IF(ISERROR(VLOOKUP(A8,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="D9" t="b">
+        <f>IF(ISERROR(VLOOKUP(A9,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="D10" t="b">
+        <f>IF(ISERROR(VLOOKUP(A10,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="D11" t="b">
+        <f>IF(ISERROR(VLOOKUP(A11,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="D12" t="b">
+        <f>IF(ISERROR(VLOOKUP(A12,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="D13" t="b">
+        <f>IF(ISERROR(VLOOKUP(A13,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="D14" t="b">
+        <f>IF(ISERROR(VLOOKUP(A14,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="D15" t="b">
+        <f>IF(ISERROR(VLOOKUP(A15,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="D16" t="b">
+        <f>IF(ISERROR(VLOOKUP(A16,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="D17" t="b">
+        <f>IF(ISERROR(VLOOKUP(A17,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="B17" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>316</v>
       </c>
       <c r="B18" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="b">
+        <f>IF(ISERROR(VLOOKUP(A18,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B19" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="b">
+        <f>IF(ISERROR(VLOOKUP(A19,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B20" t="s">
+        <v>327</v>
+      </c>
+      <c r="D20" t="b">
+        <f>IF(ISERROR(VLOOKUP(A20,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>324</v>
+      <c r="D21" t="b">
+        <f>IF(ISERROR(VLOOKUP(A21,column_name,1,FALSE)),FALSE,TRUE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D21">
+    <sortCondition descending="1" ref="D2:D21"/>
+    <sortCondition ref="A2:A21"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:A21">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>D2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>